<commit_message>
Updated the scrum list and making a few changes to the Cranium class
the summary says it all
</commit_message>
<xml_diff>
--- a/scrum list.xlsx
+++ b/scrum list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>The list of needs</t>
   </si>
@@ -53,18 +53,12 @@
     <t>Dice Rolling Animation</t>
   </si>
   <si>
-    <t>Board GUI</t>
-  </si>
-  <si>
     <t>Cards Display GUI</t>
   </si>
   <si>
     <t>Card Class creation</t>
   </si>
   <si>
-    <t xml:space="preserve">Card Library made for each color </t>
-  </si>
-  <si>
     <t>timer for each round</t>
   </si>
   <si>
@@ -84,6 +78,63 @@
   </si>
   <si>
     <t xml:space="preserve">Spaces class </t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Card Library  </t>
+  </si>
+  <si>
+    <t>Cards of each color and kind made</t>
+  </si>
+  <si>
+    <t>make a GUI that displays a square that changes colors a few times over an interval and stops on the color corresponding to the random number generated by the function to find dice results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create an example of each of the different kinds of cards for each of the colors, only one of each for now. </t>
+  </si>
+  <si>
+    <t>Create a timer that will display the seconds left in a round and then when the timer runs out, trigger then end of a round of play</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display the score for each player at the top of the Board GUI in a banner </t>
+  </si>
+  <si>
+    <t>Create a user interface that allows the players to select their game piece when the game begins, starting with the player selected to go first.</t>
+  </si>
+  <si>
+    <t>create a function that will control the order of the players turns</t>
+  </si>
+  <si>
+    <t>after placing the game board background image, find the locations that will be mapped to the spaces the pieces need to go to in order to position the players tokens onto the correct spaces.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create an object to store the values of color and graphical location of a specific space so that the board can be hardcoded with values and stored as an array of these objects. </t>
+  </si>
+  <si>
+    <t>create a gui that displays the board, timer, score, and player positions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create a new frame to display the card currently being played. </t>
+  </si>
+  <si>
+    <t>create a class to assist in presenting the Card GUI with a single object that a display interface can then be called to display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Card display Interface </t>
+  </si>
+  <si>
+    <t xml:space="preserve">create an interface to be able to display the different kinds of cars with a single method call to ease code use </t>
+  </si>
+  <si>
+    <t>create an array of each color to serve as the "deck" for the player to pull a card from at random</t>
+  </si>
+  <si>
+    <t>random card selector</t>
+  </si>
+  <si>
+    <t>given a color, select a random card from that given color type</t>
   </si>
 </sst>
 </file>
@@ -114,7 +165,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -243,12 +294,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -261,25 +385,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -596,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J17"/>
+  <dimension ref="B1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,283 +729,349 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="61.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="2:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="4"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="2:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G3" s="5"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="2:10" ht="162" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H4" s="1"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="2:10" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H5" s="1"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="2:10" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="6" t="s">
+      <c r="H6" s="1"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="2:10" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="2:10" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="2:10" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="2:10" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11" spans="2:10" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="2:10" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="2:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="6" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="2:10" ht="130.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="6" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="2:10" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="2:10" ht="160.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="2:10" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="2:9" ht="156" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="6"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="10"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="6"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="7"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="65">
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
+  <mergeCells count="73">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
     <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
     <mergeCell ref="H9:I9"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Assigned the rest of the scrum list to people who did not pick their own
And I put in the code to finish making the timer to close out the
window when completed.
</commit_message>
<xml_diff>
--- a/scrum list.xlsx
+++ b/scrum list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wraith40k\Documents\GitHub\Team14_Cranium\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>The list of needs</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Joan</t>
+  </si>
+  <si>
+    <t>courtney</t>
   </si>
 </sst>
 </file>
@@ -317,24 +320,28 @@
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -342,15 +349,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,7 +671,7 @@
   <dimension ref="B1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:E10"/>
+      <selection activeCell="B1" sqref="B1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="15" customHeight="1"/>
@@ -681,284 +684,294 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="61.5" customHeight="1">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="2:9" ht="45" customHeight="1">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="12" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="12" t="s">
+      <c r="G2" s="15"/>
+      <c r="H2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="13"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" spans="2:9" ht="123.75" customHeight="1">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="2:9" ht="162" customHeight="1">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="2:9" ht="67.5" customHeight="1">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="2:9" ht="93" customHeight="1">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
+      <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="E6" s="3"/>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="5"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="2:9" ht="93" customHeight="1">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="5"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="2:9" ht="109.5" customHeight="1">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="9" t="s">
         <v>17</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="2:9" ht="109.5" customHeight="1">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="3"/>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="2:9" ht="87" customHeight="1">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="9" t="s">
         <v>21</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" spans="2:9" ht="100.5" customHeight="1">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="5"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="2:9" ht="57.75" customHeight="1">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="5"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="2:9" ht="130.5" customHeight="1">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
+      <c r="D13" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="9" t="s">
         <v>28</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="5"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="2:9" ht="68.25" customHeight="1">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="9" t="s">
         <v>30</v>
       </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="5"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="2:9" ht="159.75" customHeight="1">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="5"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="2:9" ht="102.75" customHeight="1">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="2:9" ht="156" customHeight="1">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="9" t="s">
         <v>36</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="5"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="2:9" ht="14.25" customHeight="1">
-      <c r="B18" s="2"/>
+      <c r="B18" s="4"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="2"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="2"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="5"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="7"/>
     </row>
     <row r="19" spans="2:9" ht="14.25" customHeight="1">
-      <c r="B19" s="16"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="17"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="2:9" ht="14.25" customHeight="1">
       <c r="C20" s="1"/>
@@ -3905,6 +3918,63 @@
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F13:G13"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D18:E18"/>
@@ -3921,63 +3991,6 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cards and "Card Deck" complete
</commit_message>
<xml_diff>
--- a/scrum list.xlsx
+++ b/scrum list.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wraith40k\Documents\GitHub\Team14_Cranium\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="20496" windowHeight="7536"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="23040" windowHeight="9216"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>The list of needs</t>
   </si>
@@ -72,9 +72,6 @@
     <t xml:space="preserve">Card Library  </t>
   </si>
   <si>
-    <t>create an array of each color to serve as the "deck" for the player to pull a card from at random</t>
-  </si>
-  <si>
     <t>random card selector</t>
   </si>
   <si>
@@ -145,13 +142,28 @@
   </si>
   <si>
     <t>starting now</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">create an array of each color to serve as the "deck" for the player to pull a card from at random </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>EDIT: I went ahead and created a modified Card.java class with a display interface and how I think the whole "deck array" should be implemented. I know Courtney is in charge of the card display but I created my own simple version for testing so I'm gonna upload it in case you guys want to use it.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -166,6 +178,19 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -323,27 +348,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -351,15 +380,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:G3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="15" customHeight="1"/>
@@ -690,304 +718,308 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="61.5" customHeight="1">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="2:9" ht="45" customHeight="1">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="12" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="12" t="s">
+      <c r="G2" s="15"/>
+      <c r="H2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="13"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" spans="2:9" ht="123.75" customHeight="1">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="2:9" ht="162" customHeight="1">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="2:9" ht="67.5" customHeight="1">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="2:9" ht="93" customHeight="1">
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="2:9" ht="93" customHeight="1">
+      <c r="B7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="2:9" ht="131.4" customHeight="1">
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="2:9" ht="93" customHeight="1">
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4" t="s">
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="2:9" ht="109.5" customHeight="1">
+      <c r="B9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="2:9" ht="87" customHeight="1">
+      <c r="B10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="2:9" ht="93" customHeight="1">
-      <c r="B7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4" t="s">
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="2:9" ht="100.5" customHeight="1">
+      <c r="B11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="2:9" ht="109.5" customHeight="1">
-      <c r="B8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="2:9" ht="109.5" customHeight="1">
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="2:9" ht="87" customHeight="1">
-      <c r="B10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="2:9" ht="100.5" customHeight="1">
-      <c r="B11" s="2" t="s">
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="2:9" ht="57.75" customHeight="1">
+      <c r="B12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="4" t="s">
+      <c r="E12" s="3"/>
+      <c r="F12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="2:9" ht="130.5" customHeight="1">
+      <c r="B13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="2:9" ht="57.75" customHeight="1">
-      <c r="B12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="4" t="s">
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="2:9" ht="68.25" customHeight="1">
+      <c r="B14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="2:9" ht="130.5" customHeight="1">
-      <c r="B13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="2:9" ht="68.25" customHeight="1">
-      <c r="B14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="6" t="s">
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="2:9" ht="159.75" customHeight="1">
+      <c r="B15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="2:9" ht="159.75" customHeight="1">
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="6" t="s">
+      <c r="G15" s="3"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="2:9" ht="102.75" customHeight="1">
+      <c r="B16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="2:9" ht="102.75" customHeight="1">
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="6" t="s">
+      <c r="G16" s="3"/>
+      <c r="H16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="2:9" ht="156" customHeight="1">
+      <c r="B17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="2:9" ht="156" customHeight="1">
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="5"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="2:9" ht="14.25" customHeight="1">
-      <c r="B18" s="2"/>
+      <c r="B18" s="4"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="2"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="2"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="5"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="7"/>
     </row>
     <row r="19" spans="2:9" ht="14.25" customHeight="1">
-      <c r="B19" s="16"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="17"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="2:9" ht="14.25" customHeight="1">
       <c r="C20" s="1"/>
@@ -3934,6 +3966,63 @@
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F13:G13"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D18:E18"/>
@@ -3950,64 +4039,8 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>